<commit_message>
day of getting data from api corrected
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Лазиза</t>
+          <t>Sadikov Anvar</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -469,637 +469,367 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+998936409999</t>
+          <t>+998946045808</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sunnatbek Abdurazzokov</t>
+          <t>Muhammad</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>220000</v>
+        <v>180000</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>+998900291917</t>
+          <t>+998903203636</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Elyor</t>
+          <t>Асадбек</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>130000</v>
+        <v>320000</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+998901394848</t>
+          <t>+998970353930</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Фирдавс</t>
+          <t>Muhammadali</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>350000</v>
+        <v>300000</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+998958057777</t>
+          <t>+998977538191</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Шухрат</t>
+          <t>Малика Бадридинова</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>220000</v>
+        <v>320000</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+998998339073</t>
+          <t>+998933833036</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Nodir</t>
+          <t>Nozim</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>120000</v>
+        <v>320000</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>+998909976210</t>
+          <t>+998990833333</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sardorbek</t>
+          <t>Азиза</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>320000</v>
+        <v>1200000</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>+998997205868</t>
+          <t>+998900655055</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Саидбек</t>
+          <t>Шахзод</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>+998977427755</t>
+          <t>+998981223322</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Мадина</t>
+          <t>Мухаммадамин</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>390000</v>
+        <v>1100000</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>+998998045636</t>
+          <t>+998979979191</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Туйчиев Бунёд</t>
+          <t>Мухлиса</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>120000</v>
+        <v>150000</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>+998970020939</t>
+          <t>+998981602444</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Жахонгир</t>
+          <t>Миромон</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>370000</v>
+        <v>380000</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>+998900271700</t>
+          <t>+998998351771</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Асилбек</t>
+          <t>Абдурашид</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>220000</v>
+        <v>320000</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>+998941797077</t>
+          <t>+998957704244</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Maftuna</t>
+          <t xml:space="preserve">Бегзод </t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>120000</v>
+        <v>750000</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>+998970059105</t>
+          <t>+998977760464</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Мухлиса</t>
+          <t>Sultanova Muborak</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>320000</v>
+        <v>150000</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>+998900381242</t>
+          <t>+998993656050</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Дилафруз</t>
+          <t>Gulirano</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>350000</v>
+        <v>120000</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>+998901752606</t>
+          <t>+998958185775</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Rasulov Javohir</t>
+          <t>Raximov Muhammadjon</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>350000</v>
+        <v>320000</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>+998946960011</t>
+          <t>+998990390088</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Дилшода </t>
+          <t>Наима</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>580000</v>
+        <v>400000</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>+998903470804</t>
+          <t>+998977283121</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Гульчехра </t>
+          <t>Амаль</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>350000</v>
+        <v>320000</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>+998990016668</t>
+          <t>+998959009050</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Нодира</t>
+          <t>Nodir Qahramonov</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>200000</v>
+        <v>300000</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>+998935488777</t>
+          <t>+998915383553</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ильвина</t>
+          <t>виталий</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>120000</v>
+        <v>300000</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>+998934472545</t>
+          <t>+998949446754</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Наима</t>
+          <t>Комрон</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>420000</v>
+        <v>300000</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>+998917977320</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Нуриддин</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="n">
-        <v>350000</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>+998993654420</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Мирзиёд</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="n">
-        <v>280000</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>+998991110101</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Диор</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" t="n">
-        <v>450000</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>+998958908778</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Эльёр</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" t="n">
-        <v>150000</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>+998998946494</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>набиева парвина</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="n">
-        <v>300000</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>+998946719292</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Асилбек </t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" t="n">
-        <v>300000</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>+998946410101</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Малика</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" t="n">
-        <v>380000</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>+998994177775</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Давлатова Согдиана</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" t="n">
-        <v>300000</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>+998912803939</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>To'lqinov Elmurodjon</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="n">
-        <v>130000</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>+998932345454</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Пак Елена Львовна</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" t="n">
-        <v>350000</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>+998998109501</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Мафтуна </t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" t="n">
-        <v>300000</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>+998972391000</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Хуршид </t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" t="n">
-        <v>350000</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>+998911900699</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Allaberdiyeva Akjemal</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="n">
-        <v>220000</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>+998958502222</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Карина</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" t="n">
-        <v>130000</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>+998903193887</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Алиев хаял</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" t="n">
-        <v>130000</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>+998930003003</t>
+          <t>+998992132213</t>
         </is>
       </c>
     </row>

</xml_diff>